<commit_message>
added brand profitability analysis
</commit_message>
<xml_diff>
--- a/sheets/qtr_5/BrandProfitability-Q4.xlsx
+++ b/sheets/qtr_5/BrandProfitability-Q4.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyote\Documents\Cresicor\Project\capstone\python-analysis\sheets\qtr_5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{9FC311C3-D2C4-47A5-97D4-89561755452E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Brand Profitability" sheetId="1" r:id="rId4"/>
+    <sheet name="Brand Profitability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="TitleRegion1.A2.D15.1">'Brand Profitability'!A2</definedName>
-  </definedNames>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t>Brand Profitability</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Report Item</t>
   </si>
@@ -43,9 +44,6 @@
     <t>- Cost of Goods Sold</t>
   </si>
   <si>
-    <t>= Gross Profit</t>
-  </si>
-  <si>
     <t>Brand Design</t>
   </si>
   <si>
@@ -61,9 +59,6 @@
     <t>+ Internet Marketing</t>
   </si>
   <si>
-    <t>= Expenses</t>
-  </si>
-  <si>
     <t>Brand Profit</t>
   </si>
   <si>
@@ -74,49 +69,43 @@
   </si>
   <si>
     <t>End of Worksheet</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>Expenses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,46 +113,69 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="3" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="3" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="3" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -301,7 +313,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -312,31 +323,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -358,7 +369,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -416,7 +427,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -429,13 +440,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -453,242 +463,225 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="32" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" s="4">
+        <v>315358</v>
+      </c>
+      <c r="C2" s="4">
+        <v>144962</v>
+      </c>
+      <c r="D2" s="4">
+        <v>73752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>315358.0</v>
-      </c>
-      <c r="C3">
-        <v>144962.0</v>
-      </c>
-      <c r="D3">
-        <v>73752.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3610</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>0.0</v>
-      </c>
-      <c r="C4">
-        <v>3610.0</v>
-      </c>
-      <c r="D4">
-        <v>2000.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="4">
+        <v>136574.48280999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>61190.784370000001</v>
+      </c>
+      <c r="D4" s="4">
+        <v>40604.473230000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6">
+        <v>178783.51719000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>80161.215630000006</v>
+      </c>
+      <c r="D5" s="6">
+        <v>31147.52677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>136574.48281</v>
-      </c>
-      <c r="C5">
-        <v>61190.78437</v>
-      </c>
-      <c r="D5">
-        <v>40604.47323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
-        <v>178783.51719</v>
-      </c>
-      <c r="C6" s="5">
-        <v>80161.21563</v>
-      </c>
-      <c r="D6" s="5">
-        <v>31147.52677</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="4">
+        <v>12000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>12000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>30000</v>
-      </c>
-      <c r="D7">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="4">
+        <v>31590</v>
+      </c>
+      <c r="C8" s="4">
+        <v>49608</v>
+      </c>
+      <c r="D8" s="4">
+        <v>26531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>12000</v>
-      </c>
-      <c r="C8">
-        <v>12000</v>
-      </c>
-      <c r="D8">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="4">
+        <v>400</v>
+      </c>
+      <c r="C9" s="4">
+        <v>400</v>
+      </c>
+      <c r="D9" s="4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>31590.0</v>
-      </c>
-      <c r="C9">
-        <v>49608.0</v>
-      </c>
-      <c r="D9">
-        <v>26531.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="4">
+        <v>1904</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1904</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45894</v>
+      </c>
+      <c r="C11" s="6">
+        <v>93912</v>
+      </c>
+      <c r="D11" s="6">
+        <v>70835</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>400</v>
-      </c>
-      <c r="C10">
-        <v>400</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="6">
+        <v>132889.51719000001</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-13750.784369999999</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-39687.473230000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>1904.0</v>
-      </c>
-      <c r="C11">
-        <v>1904.0</v>
-      </c>
-      <c r="D11">
-        <v>1904.0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
+      <c r="B13" s="6">
+        <v>386</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-103</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5">
-        <v>45894.0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>93912.0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>70835.0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="4">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>-54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5">
-        <v>132889.51719</v>
-      </c>
-      <c r="C13" s="5">
-        <v>-13750.78437</v>
-      </c>
-      <c r="D13" s="5">
-        <v>-39687.47323</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5">
-        <v>386.0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>-103.0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>-709.0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <v>42.0</v>
-      </c>
-      <c r="C15">
-        <v>-9.0</v>
-      </c>
-      <c r="D15">
-        <v>-54.0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="6" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>